<commit_message>
08-DEC-2023, PDF Report Print OK by IActionResult()
</commit_message>
<xml_diff>
--- a/AppliedTax/wwwroot/PrintReports/TaxSample.xlsx
+++ b/AppliedTax/wwwroot/PrintReports/TaxSample.xlsx
@@ -358,7 +358,7 @@
       </c>
       <c s="2" t="inlineStr" r="J5">
         <is>
-          <t xml:space="preserve">101</t>
+          <t xml:space="preserve">89810</t>
         </is>
       </c>
       <c s="2" t="inlineStr" r="N5">
@@ -367,7 +367,7 @@
         </is>
       </c>
       <c s="3" r="R5">
-        <v>45231</v>
+        <v>44930</v>
       </c>
     </row>
     <row r="6" ht="6.95" customHeight="1"/>
@@ -379,7 +379,7 @@
       </c>
       <c s="2" t="inlineStr" r="J7">
         <is>
-          <t xml:space="preserve">201</t>
+          <t xml:space="preserve">256208</t>
         </is>
       </c>
       <c s="2" t="inlineStr" r="N7">
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c s="3" r="R7">
-        <v>45235</v>
+        <v>45029</v>
       </c>
     </row>
     <row r="8" ht="7.05" customHeight="1"/>
@@ -445,18 +445,18 @@
       <c s="8" t="str" r="B11"/>
       <c s="5" t="str" r="C11"/>
       <c s="9" r="D11">
-        <v>20</v>
+        <v>203</v>
       </c>
       <c s="7" t="str" r="E11"/>
       <c s="5" t="str" r="F11"/>
       <c s="10" r="G11">
-        <v>13</v>
+        <v>5203</v>
       </c>
       <c s="7" t="str" r="H11"/>
       <c s="7" t="str" r="I11"/>
       <c s="5" t="str" r="J11"/>
       <c s="9" r="K11">
-        <v>260</v>
+        <v>1056209</v>
       </c>
       <c s="5" t="str" r="L11"/>
       <c s="10" r="M11">
@@ -464,54 +464,86 @@
       </c>
       <c s="5" t="str" r="N11"/>
       <c s="9" r="O11">
-        <v>2.6</v>
+        <v>266.5</v>
       </c>
       <c s="7" t="str" r="P11"/>
       <c s="7" t="str" r="Q11"/>
       <c s="5" t="str" r="R11"/>
       <c s="9" r="S11">
-        <v>40</v>
+        <v>7940</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="0">
-      <c s="4" t="inlineStr" r="B12">
-        <is>
-          <t xml:space="preserve">Total</t>
-        </is>
-      </c>
+      <c s="8" t="str" r="B12"/>
       <c s="5" t="str" r="C12"/>
-      <c s="11" r="D12">
-        <v>20</v>
+      <c s="9" r="D12">
+        <v>50</v>
       </c>
       <c s="7" t="str" r="E12"/>
       <c s="5" t="str" r="F12"/>
-      <c s="12" r="G12">
-        <v>13</v>
+      <c s="10" r="G12">
+        <v>20</v>
       </c>
       <c s="7" t="str" r="H12"/>
       <c s="7" t="str" r="I12"/>
       <c s="5" t="str" r="J12"/>
-      <c s="11" r="K12">
-        <v>260</v>
+      <c s="9" r="K12">
+        <v>1000</v>
       </c>
       <c s="5" t="str" r="L12"/>
-      <c s="13" t="inlineStr" r="M12">
-        <is>
-          <t xml:space="preserve"/>
-        </is>
+      <c s="10" r="M12">
+        <v>13</v>
       </c>
       <c s="5" t="str" r="N12"/>
-      <c s="11" r="O12">
-        <v>20</v>
+      <c s="9" r="O12">
+        <v>130</v>
       </c>
       <c s="7" t="str" r="P12"/>
       <c s="7" t="str" r="Q12"/>
       <c s="5" t="str" r="R12"/>
-      <c s="11" r="S12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" ht="1" customHeight="1"/>
+      <c s="9" r="S12">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="13" ht="18" customHeight="0">
+      <c s="4" t="inlineStr" r="B13">
+        <is>
+          <t xml:space="preserve">Total</t>
+        </is>
+      </c>
+      <c s="5" t="str" r="C13"/>
+      <c s="11" r="D13">
+        <v>253</v>
+      </c>
+      <c s="7" t="str" r="E13"/>
+      <c s="5" t="str" r="F13"/>
+      <c s="12" r="G13">
+        <v>5223</v>
+      </c>
+      <c s="7" t="str" r="H13"/>
+      <c s="7" t="str" r="I13"/>
+      <c s="5" t="str" r="J13"/>
+      <c s="11" r="K13">
+        <v>1057209</v>
+      </c>
+      <c s="5" t="str" r="L13"/>
+      <c s="13" t="inlineStr" r="M13">
+        <is>
+          <t xml:space="preserve"/>
+        </is>
+      </c>
+      <c s="5" t="str" r="N13"/>
+      <c s="11" r="O13">
+        <v>18890</v>
+      </c>
+      <c s="7" t="str" r="P13"/>
+      <c s="7" t="str" r="Q13"/>
+      <c s="5" t="str" r="R13"/>
+      <c s="11" r="S13">
+        <v>20520</v>
+      </c>
+    </row>
+    <row r="14" ht="1" customHeight="1"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="C2:D7"/>
@@ -542,11 +574,17 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="O12:R12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:R13"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="1.0729200787401576" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Segoe UI,Bold Italic"&amp;8 Powered by Applied Software House &amp;R&amp;"Segoe UI,Italic"&amp;8 12/1/2023 11:09:10 PM </oddFooter>
+    <oddFooter>&amp;L&amp;"Segoe UI,Bold Italic"&amp;8 Powered by Applied Software House &amp;R&amp;"Segoe UI,Italic"&amp;8 2023-12-08 9:42:27 AM </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>
 </worksheet>

</xml_diff>

<commit_message>
SA 11-DEC-2023, PFD Is being opened in new tab. ok
</commit_message>
<xml_diff>
--- a/AppliedTax/wwwroot/PrintReports/TaxSample.xlsx
+++ b/AppliedTax/wwwroot/PrintReports/TaxSample.xlsx
@@ -358,7 +358,7 @@
       </c>
       <c s="2" t="inlineStr" r="J5">
         <is>
-          <t xml:space="preserve">89810</t>
+          <t xml:space="preserve">931</t>
         </is>
       </c>
       <c s="2" t="inlineStr" r="N5">
@@ -367,7 +367,7 @@
         </is>
       </c>
       <c s="3" r="R5">
-        <v>44930</v>
+        <v>44958</v>
       </c>
     </row>
     <row r="6" ht="6.95" customHeight="1"/>
@@ -379,7 +379,7 @@
       </c>
       <c s="2" t="inlineStr" r="J7">
         <is>
-          <t xml:space="preserve">256208</t>
+          <t xml:space="preserve">8896</t>
         </is>
       </c>
       <c s="2" t="inlineStr" r="N7">
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c s="3" r="R7">
-        <v>45029</v>
+        <v>44993</v>
       </c>
     </row>
     <row r="8" ht="7.05" customHeight="1"/>
@@ -445,18 +445,18 @@
       <c s="8" t="str" r="B11"/>
       <c s="5" t="str" r="C11"/>
       <c s="9" r="D11">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c s="7" t="str" r="E11"/>
       <c s="5" t="str" r="F11"/>
       <c s="10" r="G11">
-        <v>5203</v>
+        <v>12</v>
       </c>
       <c s="7" t="str" r="H11"/>
       <c s="7" t="str" r="I11"/>
       <c s="5" t="str" r="J11"/>
       <c s="9" r="K11">
-        <v>1056209</v>
+        <v>1476</v>
       </c>
       <c s="5" t="str" r="L11"/>
       <c s="10" r="M11">
@@ -464,31 +464,31 @@
       </c>
       <c s="5" t="str" r="N11"/>
       <c s="9" r="O11">
-        <v>266.5</v>
+        <v>191.88</v>
       </c>
       <c s="7" t="str" r="P11"/>
       <c s="7" t="str" r="Q11"/>
       <c s="5" t="str" r="R11"/>
       <c s="9" r="S11">
-        <v>7940</v>
+        <v>20664</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="0">
       <c s="8" t="str" r="B12"/>
       <c s="5" t="str" r="C12"/>
       <c s="9" r="D12">
-        <v>50</v>
+        <v>1234</v>
       </c>
       <c s="7" t="str" r="E12"/>
       <c s="5" t="str" r="F12"/>
       <c s="10" r="G12">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c s="7" t="str" r="H12"/>
       <c s="7" t="str" r="I12"/>
       <c s="5" t="str" r="J12"/>
       <c s="9" r="K12">
-        <v>1000</v>
+        <v>396114</v>
       </c>
       <c s="5" t="str" r="L12"/>
       <c s="10" r="M12">
@@ -496,54 +496,150 @@
       </c>
       <c s="5" t="str" r="N12"/>
       <c s="9" r="O12">
-        <v>130</v>
+        <v>51494.82</v>
       </c>
       <c s="7" t="str" r="P12"/>
       <c s="7" t="str" r="Q12"/>
       <c s="5" t="str" r="R12"/>
       <c s="9" r="S12">
-        <v>14000</v>
+        <v>396117</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="0">
-      <c s="4" t="inlineStr" r="B13">
-        <is>
-          <t xml:space="preserve">Total</t>
-        </is>
-      </c>
+      <c s="8" t="str" r="B13"/>
       <c s="5" t="str" r="C13"/>
-      <c s="11" r="D13">
-        <v>253</v>
+      <c s="9" r="D13">
+        <v>200</v>
       </c>
       <c s="7" t="str" r="E13"/>
       <c s="5" t="str" r="F13"/>
-      <c s="12" r="G13">
-        <v>5223</v>
+      <c s="10" r="G13">
+        <v>2</v>
       </c>
       <c s="7" t="str" r="H13"/>
       <c s="7" t="str" r="I13"/>
       <c s="5" t="str" r="J13"/>
-      <c s="11" r="K13">
-        <v>1057209</v>
+      <c s="9" r="K13">
+        <v>400</v>
       </c>
       <c s="5" t="str" r="L13"/>
-      <c s="13" t="inlineStr" r="M13">
-        <is>
-          <t xml:space="preserve"/>
-        </is>
+      <c s="10" r="M13">
+        <v>13</v>
       </c>
       <c s="5" t="str" r="N13"/>
-      <c s="11" r="O13">
-        <v>18890</v>
+      <c s="9" r="O13">
+        <v>52</v>
       </c>
       <c s="7" t="str" r="P13"/>
       <c s="7" t="str" r="Q13"/>
       <c s="5" t="str" r="R13"/>
-      <c s="11" r="S13">
-        <v>20520</v>
-      </c>
-    </row>
-    <row r="14" ht="1" customHeight="1"/>
+      <c s="9" r="S13">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="0">
+      <c s="8" t="str" r="B14"/>
+      <c s="5" t="str" r="C14"/>
+      <c s="9" r="D14">
+        <v>3</v>
+      </c>
+      <c s="7" t="str" r="E14"/>
+      <c s="5" t="str" r="F14"/>
+      <c s="10" r="G14">
+        <v>3</v>
+      </c>
+      <c s="7" t="str" r="H14"/>
+      <c s="7" t="str" r="I14"/>
+      <c s="5" t="str" r="J14"/>
+      <c s="9" r="K14">
+        <v>9</v>
+      </c>
+      <c s="5" t="str" r="L14"/>
+      <c s="10" r="M14">
+        <v>13</v>
+      </c>
+      <c s="5" t="str" r="N14"/>
+      <c s="9" r="O14">
+        <v>1.17</v>
+      </c>
+      <c s="7" t="str" r="P14"/>
+      <c s="7" t="str" r="Q14"/>
+      <c s="5" t="str" r="R14"/>
+      <c s="9" r="S14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" ht="18" customHeight="0">
+      <c s="8" t="str" r="B15"/>
+      <c s="5" t="str" r="C15"/>
+      <c s="9" r="D15">
+        <v>5</v>
+      </c>
+      <c s="7" t="str" r="E15"/>
+      <c s="5" t="str" r="F15"/>
+      <c s="10" r="G15">
+        <v>30</v>
+      </c>
+      <c s="7" t="str" r="H15"/>
+      <c s="7" t="str" r="I15"/>
+      <c s="5" t="str" r="J15"/>
+      <c s="9" r="K15">
+        <v>150</v>
+      </c>
+      <c s="5" t="str" r="L15"/>
+      <c s="10" r="M15">
+        <v>13</v>
+      </c>
+      <c s="5" t="str" r="N15"/>
+      <c s="9" r="O15">
+        <v>19.5</v>
+      </c>
+      <c s="7" t="str" r="P15"/>
+      <c s="7" t="str" r="Q15"/>
+      <c s="5" t="str" r="R15"/>
+      <c s="9" r="S15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" ht="18" customHeight="0">
+      <c s="4" t="inlineStr" r="B16">
+        <is>
+          <t xml:space="preserve">Total</t>
+        </is>
+      </c>
+      <c s="5" t="str" r="C16"/>
+      <c s="11" r="D16">
+        <v>1565</v>
+      </c>
+      <c s="7" t="str" r="E16"/>
+      <c s="5" t="str" r="F16"/>
+      <c s="12" r="G16">
+        <v>368</v>
+      </c>
+      <c s="7" t="str" r="H16"/>
+      <c s="7" t="str" r="I16"/>
+      <c s="5" t="str" r="J16"/>
+      <c s="11" r="K16">
+        <v>398149</v>
+      </c>
+      <c s="5" t="str" r="L16"/>
+      <c s="13" t="inlineStr" r="M16">
+        <is>
+          <t xml:space="preserve"/>
+        </is>
+      </c>
+      <c s="5" t="str" r="N16"/>
+      <c s="11" r="O16">
+        <v>24417</v>
+      </c>
+      <c s="7" t="str" r="P16"/>
+      <c s="7" t="str" r="Q16"/>
+      <c s="5" t="str" r="R16"/>
+      <c s="11" r="S16">
+        <v>422537</v>
+      </c>
+    </row>
+    <row r="17" ht="1" customHeight="1"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="C2:D7"/>
@@ -580,11 +676,29 @@
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="O13:R13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:R16"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="1.0729200787401576" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Segoe UI,Bold Italic"&amp;8 Powered by Applied Software House &amp;R&amp;"Segoe UI,Italic"&amp;8 2023-12-08 9:42:27 AM </oddFooter>
+    <oddFooter>&amp;L&amp;"Segoe UI,Bold Italic"&amp;8 Powered by Applied Software House &amp;R&amp;"Segoe UI,Italic"&amp;8 2023-12-11 9:12:41 AM </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>
 </worksheet>

</xml_diff>